<commit_message>
test: add new tests and update existing tests
- Add TaxConfigRepository tests for database-backed tax configs
- Add TaxConfiguration seeder tests
- Add tax config tests (TaxIncome, TaxRealization, TaxSalary, TaxFortune)
- Add TaxTypesConfig test
- Add TaxTypeResolver unit test
- Add JsonConfigValidity, PhpVersionRequirement, ChangerateDbLookup tests
- Update existing tests to use new TaxConfigRepository
- Update test config JSON files with new structure
- Fix PSR-4 compliance for test helper classes
</commit_message>
<xml_diff>
--- a/tests/Feature/config/salary_tenpercent.xlsx
+++ b/tests/Feature/config/salary_tenpercent.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
   <si>
     <t>Sum total</t>
   </si>
@@ -180,10 +180,109 @@
     <t>private</t>
   </si>
   <si>
-    <t>income</t>
+    <t>salary</t>
   </si>
   <si>
-    <t>Income</t>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 0 skatt, Trygdeavgift 7.8% gir 0 skatt  Trinnskatt:0 snitt 0%,  Bracket0 (0&lt;)208050)0%=0</t>
+  </si>
+  <si>
+    <t>Income Fellesskatt: 22% gir 368554 skatt, Trygdeavgift 7.7% gir 139755 skatt  Trinnskatt:200516 snitt 4%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=71552</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 405409 skatt, Trygdeavgift 7.7% gir 153731 skatt  Trinnskatt:232642 snitt 5%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=103678</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 445950 skatt, Trygdeavgift 7.7% gir 169104 skatt  Trinnskatt:267980 snitt 6%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=139016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 490545 skatt, Trygdeavgift 7.7% gir 186014 skatt  Trinnskatt:306852 snitt 7%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=177888</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 539600 skatt, Trygdeavgift 7.7% gir 204615 skatt  Trinnskatt:349611 snitt 8%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=220647</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 593560 skatt, Trygdeavgift 7.7% gir 225077 skatt  Trinnskatt:396646 snitt 9%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=267682</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 652916 skatt, Trygdeavgift 7.7% gir 247584 skatt  Trinnskatt:448384 snitt 10%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=319420</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 718207 skatt, Trygdeavgift 7.7% gir 272343 skatt  Trinnskatt:505296 snitt 11%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=376332</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 790028 skatt, Trygdeavgift 7.7% gir 299577 skatt  Trinnskatt:567900 snitt 11%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=438936</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 869031 skatt, Trygdeavgift 7.7% gir 329535 skatt  Trinnskatt:636764 snitt 12%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=507800</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 955934 skatt, Trygdeavgift 7.7% gir 362488 skatt  Trinnskatt:712514 snitt 12%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=583550</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1051527 skatt, Trygdeavgift 7.7% gir 398737 skatt  Trinnskatt:795839 snitt 13%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=666875</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1156680 skatt, Trygdeavgift 7.7% gir 438611 skatt  Trinnskatt:887497 snitt 13%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=758533</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1272348 skatt, Trygdeavgift 7.7% gir 482472 skatt  Trinnskatt:988321 snitt 14%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=859357</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1399583 skatt, Trygdeavgift 7.7% gir 530719 skatt  Trinnskatt:1099227 snitt 14%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=970263</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1539541 skatt, Trygdeavgift 7.7% gir 583791 skatt  Trinnskatt:1221223 snitt 14%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=1092259</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1693495 skatt, Trygdeavgift 7.7% gir 642170 skatt  Trinnskatt:1355419 snitt 15%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=1226455</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 1862845 skatt, Trygdeavgift 7.7% gir 706388 skatt  Trinnskatt:1503035 snitt 15%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=1374071</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 2049130 skatt, Trygdeavgift 7.7% gir 777026 skatt  Trinnskatt:1665413 snitt 15%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=1536449</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 2254043 skatt, Trygdeavgift 7.7% gir 854729 skatt  Trinnskatt:1844028 snitt 15%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=1715064</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 2479447 skatt, Trygdeavgift 7.7% gir 940202 skatt  Trinnskatt:2040505 snitt 16%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=1911541</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 2727391 skatt, Trygdeavgift 7.7% gir 1034222 skatt  Trinnskatt:2256629 snitt 16%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=2127665</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 3000131 skatt, Trygdeavgift 7.7% gir 1137644 skatt  Trinnskatt:2494366 snitt 16%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=2365402</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 3300144 skatt, Trygdeavgift 7.7% gir 1251409 skatt  Trinnskatt:2755876 snitt 16%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=2626912</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 3630158 skatt, Trygdeavgift 7.7% gir 1376550 skatt  Trinnskatt:3043538 snitt 16%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=2914574</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 3993174 skatt, Trygdeavgift 7.7% gir 1514205 skatt  Trinnskatt:3359965 snitt 16%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=3231001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 4392491 skatt, Trygdeavgift 7.7% gir 1665625 skatt  Trinnskatt:3708036 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=3579072</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 4831741 skatt, Trygdeavgift 7.7% gir 1832188 skatt  Trinnskatt:4090913 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=3961949</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 5314915 skatt, Trygdeavgift 7.7% gir 2015406 skatt  Trinnskatt:4512079 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=4383115</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 5846407 skatt, Trygdeavgift 7.7% gir 2216947 skatt  Trinnskatt:4975361 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=4846397</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 6431047 skatt, Trygdeavgift 7.7% gir 2438642 skatt  Trinnskatt:5484971 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=5356007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 7074152 skatt, Trygdeavgift 7.7% gir 2682506 skatt  Trinnskatt:6045541 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=5916577</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fellesskatt: 22% gir 7781567 skatt, Trygdeavgift 7.7% gir 2950757 skatt  Trinnskatt:6662169 snitt 17%,  Bracket0 (217400)0%=0, Bracket1 (306050)1.7%=1507, Bracket2 (697150)4%=15644, Bracket3 (942400)13.7%=33599, Bracket4 (1410750)16.7%=78214, Bracket5 (&gt;1410750)17.7%=6533205</t>
   </si>
 </sst>
 </file>
@@ -638,7 +737,7 @@
     <col min="4" max="4" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
@@ -992,9 +1091,11 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="10"/>
+        <v>708825.0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.39053719008264</v>
+      </c>
       <c r="I7" s="9">
         <v>0</v>
       </c>
@@ -1054,10 +1155,10 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="9">
-        <v>1815000.0</v>
+        <v>1106175.0</v>
       </c>
       <c r="AJ7" s="9">
-        <v>1815000.0</v>
+        <v>1106175.0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="9">
@@ -1091,9 +1192,11 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>791782.0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.39658502379164</v>
+      </c>
       <c r="I8" s="2">
         <v>0</v>
       </c>
@@ -1153,10 +1256,10 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="7">
-        <v>1996500.0</v>
+        <v>1204718.0</v>
       </c>
       <c r="AJ8" s="2">
-        <v>3811500.0</v>
+        <v>2310893.0</v>
       </c>
       <c r="AK8" s="3"/>
       <c r="AL8" s="2">
@@ -1190,9 +1293,11 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>883034.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.40208273569656</v>
+      </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
@@ -1252,10 +1357,10 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="7">
-        <v>2196150.0</v>
+        <v>1313116.0</v>
       </c>
       <c r="AJ9" s="2">
-        <v>6007650.0</v>
+        <v>3624009.0</v>
       </c>
       <c r="AK9" s="3"/>
       <c r="AL9" s="2">
@@ -1289,9 +1394,11 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="3"/>
+        <v>983411.0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.40708057282062</v>
+      </c>
       <c r="I10" s="2">
         <v>0</v>
       </c>
@@ -1351,10 +1458,10 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="7">
-        <v>2415765.0</v>
+        <v>1432354.0</v>
       </c>
       <c r="AJ10" s="2">
-        <v>8423415.0</v>
+        <v>5056363.0</v>
       </c>
       <c r="AK10" s="3"/>
       <c r="AL10" s="2">
@@ -1388,9 +1495,11 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>1093826.0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.41162417401</v>
+      </c>
       <c r="I11" s="2">
         <v>0</v>
       </c>
@@ -1450,10 +1559,10 @@
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="7">
-        <v>2657341.5</v>
+        <v>1563515.5</v>
       </c>
       <c r="AJ11" s="2">
-        <v>11080756.5</v>
+        <v>6619878.5</v>
       </c>
       <c r="AK11" s="3"/>
       <c r="AL11" s="2">
@@ -1487,9 +1596,11 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>1215283.0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.41575481337093</v>
+      </c>
       <c r="I12" s="2">
         <v>0</v>
       </c>
@@ -1549,10 +1660,10 @@
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="7">
-        <v>2923076.2</v>
+        <v>1707793.2</v>
       </c>
       <c r="AJ12" s="2">
-        <v>14003832.7</v>
+        <v>8327671.7</v>
       </c>
       <c r="AK12" s="3"/>
       <c r="AL12" s="2">
@@ -1586,9 +1697,11 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>1348884.0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.41950951046712</v>
+      </c>
       <c r="I13" s="2">
         <v>0</v>
       </c>
@@ -1648,10 +1761,10 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="7">
-        <v>3215383.6</v>
+        <v>1866499.6</v>
       </c>
       <c r="AJ13" s="2">
-        <v>17219216.3</v>
+        <v>10194171.3</v>
       </c>
       <c r="AK13" s="3"/>
       <c r="AL13" s="2">
@@ -1685,9 +1798,11 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>1495846.0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.42292304744939</v>
+      </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
@@ -1747,10 +1862,10 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="7">
-        <v>3536922.4</v>
+        <v>2041076.4</v>
       </c>
       <c r="AJ14" s="2">
-        <v>20756138.7</v>
+        <v>12235247.7</v>
       </c>
       <c r="AK14" s="3"/>
       <c r="AL14" s="2">
@@ -1784,9 +1899,11 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>1657505.0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.42602656413478</v>
+      </c>
       <c r="I15" s="2">
         <v>0</v>
       </c>
@@ -1846,10 +1963,10 @@
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="7">
-        <v>3890614.2</v>
+        <v>2233109.2</v>
       </c>
       <c r="AJ15" s="2">
-        <v>24646752.9</v>
+        <v>14468356.9</v>
       </c>
       <c r="AK15" s="3"/>
       <c r="AL15" s="2">
@@ -1883,9 +2000,11 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H16" s="3"/>
+        <v>1835330.0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.42884794486984</v>
+      </c>
       <c r="I16" s="2">
         <v>0</v>
       </c>
@@ -1945,10 +2064,10 @@
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="7">
-        <v>4279675.4</v>
+        <v>2444345.4</v>
       </c>
       <c r="AJ16" s="2">
-        <v>28926428.3</v>
+        <v>16912702.3</v>
       </c>
       <c r="AK16" s="3"/>
       <c r="AL16" s="2">
@@ -1982,9 +2101,11 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H17" s="3"/>
+        <v>2030936.0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.43141253822906</v>
+      </c>
       <c r="I17" s="2">
         <v>0</v>
       </c>
@@ -2044,10 +2165,10 @@
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
       <c r="AI17" s="7">
-        <v>4707642.5</v>
+        <v>2676706.5</v>
       </c>
       <c r="AJ17" s="2">
-        <v>33634070.8</v>
+        <v>19589408.8</v>
       </c>
       <c r="AK17" s="3"/>
       <c r="AL17" s="2">
@@ -2081,9 +2202,11 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H18" s="3"/>
+        <v>2246103.0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.43374398147477</v>
+      </c>
       <c r="I18" s="2">
         <v>0</v>
       </c>
@@ -2143,10 +2266,10 @@
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="7">
-        <v>5178407.3</v>
+        <v>2932304.3</v>
       </c>
       <c r="AJ18" s="2">
-        <v>38812478.1</v>
+        <v>22521713.1</v>
       </c>
       <c r="AK18" s="3"/>
       <c r="AL18" s="2">
@@ -2180,9 +2303,11 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H19" s="3"/>
+        <v>2482788.0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.43586377046068</v>
+      </c>
       <c r="I19" s="2">
         <v>0</v>
       </c>
@@ -2242,10 +2367,10 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="7">
-        <v>5696247.7</v>
+        <v>3213459.7</v>
       </c>
       <c r="AJ19" s="2">
-        <v>44508725.8</v>
+        <v>25735172.8</v>
       </c>
       <c r="AK19" s="3"/>
       <c r="AL19" s="2">
@@ -2279,9 +2404,11 @@
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>2743141.0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.43779072565916</v>
+      </c>
       <c r="I20" s="2">
         <v>0</v>
       </c>
@@ -2341,10 +2468,10 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="7">
-        <v>6265872.8</v>
+        <v>3522731.8</v>
       </c>
       <c r="AJ20" s="2">
-        <v>50774598.6</v>
+        <v>29257904.6</v>
       </c>
       <c r="AK20" s="3"/>
       <c r="AL20" s="2">
@@ -2378,9 +2505,11 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H21" s="3"/>
+        <v>3029529.0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.43954246642523</v>
+      </c>
       <c r="I21" s="2">
         <v>0</v>
       </c>
@@ -2440,10 +2569,10 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="7">
-        <v>6892460.3</v>
+        <v>3862931.3</v>
       </c>
       <c r="AJ21" s="2">
-        <v>57667058.9</v>
+        <v>33120835.9</v>
       </c>
       <c r="AK21" s="3"/>
       <c r="AL21" s="2">
@@ -2477,9 +2606,11 @@
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H22" s="14"/>
+        <v>3344555.0</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0.44113488441783</v>
+      </c>
       <c r="I22" s="13">
         <v>0</v>
       </c>
@@ -2539,10 +2670,10 @@
       <c r="AG22" s="14"/>
       <c r="AH22" s="14"/>
       <c r="AI22" s="13">
-        <v>7581706.0</v>
+        <v>4237151.0</v>
       </c>
       <c r="AJ22" s="13">
-        <v>65248764.9</v>
+        <v>37357986.9</v>
       </c>
       <c r="AK22" s="14"/>
       <c r="AL22" s="13">
@@ -2576,9 +2707,11 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="3"/>
+        <v>3691084.0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.4425825677085</v>
+      </c>
       <c r="I23" s="2">
         <v>0</v>
       </c>
@@ -2638,10 +2771,10 @@
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
       <c r="AI23" s="7">
-        <v>8339876.6</v>
+        <v>4648792.6</v>
       </c>
       <c r="AJ23" s="2">
-        <v>73588641.5</v>
+        <v>42006779.5</v>
       </c>
       <c r="AK23" s="3"/>
       <c r="AL23" s="2">
@@ -2675,9 +2808,11 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H24" s="3"/>
+        <v>4072268.0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.44389885104802</v>
+      </c>
       <c r="I24" s="2">
         <v>0</v>
       </c>
@@ -2737,10 +2872,10 @@
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="7">
-        <v>9173864.7</v>
+        <v>5101596.7</v>
       </c>
       <c r="AJ24" s="2">
-        <v>82762506.2</v>
+        <v>47108376.2</v>
       </c>
       <c r="AK24" s="3"/>
       <c r="AL24" s="2">
@@ -2774,9 +2909,11 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>4491569.0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.44509533827395</v>
+      </c>
       <c r="I25" s="2">
         <v>0</v>
       </c>
@@ -2836,10 +2973,10 @@
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
       <c r="AI25" s="7">
-        <v>10091251.5</v>
+        <v>5599682.5</v>
       </c>
       <c r="AJ25" s="2">
-        <v>92853757.7</v>
+        <v>52708058.7</v>
       </c>
       <c r="AK25" s="3"/>
       <c r="AL25" s="2">
@@ -2873,9 +3010,11 @@
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>4952800.0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.44618303601431</v>
+      </c>
       <c r="I26" s="2">
         <v>0</v>
       </c>
@@ -2935,10 +3074,10 @@
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="7">
-        <v>11100377.2</v>
+        <v>6147577.2</v>
       </c>
       <c r="AJ26" s="2">
-        <v>103954134.9</v>
+        <v>58855635.9</v>
       </c>
       <c r="AK26" s="3"/>
       <c r="AL26" s="2">
@@ -2972,9 +3111,11 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H27" s="3"/>
+        <v>5460154.0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.44717187205771</v>
+      </c>
       <c r="I27" s="2">
         <v>0</v>
       </c>
@@ -3034,10 +3175,10 @@
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="7">
-        <v>12210414.7</v>
+        <v>6750260.7</v>
       </c>
       <c r="AJ27" s="2">
-        <v>116164549.6</v>
+        <v>65605896.6</v>
       </c>
       <c r="AK27" s="3"/>
       <c r="AL27" s="2">
@@ -3071,9 +3212,11 @@
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H28" s="3"/>
+        <v>6018242.0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.44807069136545</v>
+      </c>
       <c r="I28" s="2">
         <v>0</v>
       </c>
@@ -3133,10 +3276,10 @@
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
       <c r="AI28" s="7">
-        <v>13431456.5</v>
+        <v>7413214.5</v>
       </c>
       <c r="AJ28" s="2">
-        <v>129596006.1</v>
+        <v>73019111.1</v>
       </c>
       <c r="AK28" s="3"/>
       <c r="AL28" s="2">
@@ -3170,9 +3313,11 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="3"/>
+        <v>6632141.0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.44888794200876</v>
+      </c>
       <c r="I29" s="2">
         <v>0</v>
       </c>
@@ -3232,10 +3377,10 @@
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="7">
-        <v>14774602.7</v>
+        <v>8142461.7</v>
       </c>
       <c r="AJ29" s="2">
-        <v>144370608.8</v>
+        <v>81161572.8</v>
       </c>
       <c r="AK29" s="3"/>
       <c r="AL29" s="2">
@@ -3269,9 +3414,11 @@
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="H30" s="18"/>
+        <v>7307429.0</v>
+      </c>
+      <c r="H30" s="18">
+        <v>0.44963084779518</v>
+      </c>
       <c r="I30" s="17">
         <v>0</v>
       </c>
@@ -3331,10 +3478,10 @@
       <c r="AG30" s="18"/>
       <c r="AH30" s="18"/>
       <c r="AI30" s="17">
-        <v>16252063.3</v>
+        <v>8944634.3</v>
       </c>
       <c r="AJ30" s="17">
-        <v>160622672.1</v>
+        <v>90106207.1</v>
       </c>
       <c r="AK30" s="18"/>
       <c r="AL30" s="17">
@@ -3368,9 +3515,11 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H31" s="3"/>
+        <v>8050246.0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.45030624447773</v>
+      </c>
       <c r="I31" s="2">
         <v>0</v>
       </c>
@@ -3430,10 +3579,10 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="7">
-        <v>17877269.3</v>
+        <v>9827023.3</v>
       </c>
       <c r="AJ31" s="2">
-        <v>178499941.4</v>
+        <v>99933230.4</v>
       </c>
       <c r="AK31" s="3"/>
       <c r="AL31" s="2">
@@ -3467,9 +3616,11 @@
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>8867344.0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.45092020588725</v>
+      </c>
       <c r="I32" s="2">
         <v>0</v>
       </c>
@@ -3529,10 +3680,10 @@
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
       <c r="AI32" s="7">
-        <v>19664995.9</v>
+        <v>10797651.9</v>
       </c>
       <c r="AJ32" s="2">
-        <v>198164937.3</v>
+        <v>110730882.3</v>
       </c>
       <c r="AK32" s="3"/>
       <c r="AL32" s="2">
@@ -3566,9 +3717,11 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>9766152.0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.45147835270345</v>
+      </c>
       <c r="I33" s="2">
         <v>0</v>
       </c>
@@ -3628,10 +3781,10 @@
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="7">
-        <v>21631495.6</v>
+        <v>11865343.6</v>
       </c>
       <c r="AJ33" s="2">
-        <v>219796432.9</v>
+        <v>122596225.9</v>
       </c>
       <c r="AK33" s="3"/>
       <c r="AL33" s="2">
@@ -3665,9 +3818,11 @@
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="H34" s="18"/>
+        <v>10754842.0</v>
+      </c>
+      <c r="H34" s="18">
+        <v>0.45198580305815</v>
+      </c>
       <c r="I34" s="17">
         <v>0</v>
       </c>
@@ -3727,10 +3882,10 @@
       <c r="AG34" s="18"/>
       <c r="AH34" s="18"/>
       <c r="AI34" s="17">
-        <v>23794645.6</v>
+        <v>13039803.6</v>
       </c>
       <c r="AJ34" s="17">
-        <v>243591078.5</v>
+        <v>135636029.5</v>
       </c>
       <c r="AK34" s="18"/>
       <c r="AL34" s="17">
@@ -3764,9 +3919,11 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H35" s="3"/>
+        <v>11842400.0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.45244708334044</v>
+      </c>
       <c r="I35" s="2">
         <v>0</v>
       </c>
@@ -3826,10 +3983,10 @@
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
       <c r="AI35" s="7">
-        <v>26174110.6</v>
+        <v>14331710.6</v>
       </c>
       <c r="AJ35" s="2">
-        <v>269765189.1</v>
+        <v>149967740.1</v>
       </c>
       <c r="AK35" s="3"/>
       <c r="AL35" s="2">
@@ -3863,9 +4020,11 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H36" s="3"/>
+        <v>13038715.0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.45286647071709</v>
+      </c>
       <c r="I36" s="2">
         <v>0</v>
       </c>
@@ -3925,10 +4084,10 @@
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
       <c r="AI36" s="7">
-        <v>28791522.1</v>
+        <v>15752807.1</v>
       </c>
       <c r="AJ36" s="2">
-        <v>298556711.2</v>
+        <v>165720547.2</v>
       </c>
       <c r="AK36" s="3"/>
       <c r="AL36" s="2">
@@ -3962,9 +4121,11 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H37" s="3"/>
+        <v>14354660.0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.45324769246624</v>
+      </c>
       <c r="I37" s="2">
         <v>0</v>
       </c>
@@ -4024,10 +4185,10 @@
       <c r="AG37" s="3"/>
       <c r="AH37" s="3"/>
       <c r="AI37" s="7">
-        <v>31670674.2</v>
+        <v>17316014.2</v>
       </c>
       <c r="AJ37" s="2">
-        <v>330227385.4</v>
+        <v>183036561.4</v>
       </c>
       <c r="AK37" s="3"/>
       <c r="AL37" s="2">
@@ -4061,9 +4222,11 @@
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H38" s="3"/>
+        <v>15802199.0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0.45359424477501</v>
+      </c>
       <c r="I38" s="2">
         <v>0</v>
       </c>
@@ -4123,10 +4286,10 @@
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
       <c r="AI38" s="7">
-        <v>34837741.4</v>
+        <v>19035542.4</v>
       </c>
       <c r="AJ38" s="2">
-        <v>365065126.8</v>
+        <v>202072103.8</v>
       </c>
       <c r="AK38" s="3"/>
       <c r="AL38" s="2">
@@ -4160,9 +4323,11 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H39" s="3"/>
+        <v>17394493.0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.45390932364258</v>
+      </c>
       <c r="I39" s="2">
         <v>0</v>
       </c>
@@ -4222,10 +4387,10 @@
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
       <c r="AI39" s="7">
-        <v>38321515.1</v>
+        <v>20927022.1</v>
       </c>
       <c r="AJ39" s="2">
-        <v>403386641.9</v>
+        <v>222999125.9</v>
       </c>
       <c r="AK39" s="3"/>
       <c r="AL39" s="2">
@@ -4402,7 +4567,7 @@
     <col min="4" max="4" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
@@ -4756,9 +4921,11 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="10"/>
+        <v>708825.0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.39053719008264</v>
+      </c>
       <c r="I7" s="9">
         <v>0</v>
       </c>
@@ -4818,10 +4985,10 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="9">
-        <v>1815000.0</v>
+        <v>1106175.0</v>
       </c>
       <c r="AJ7" s="9">
-        <v>1815000.0</v>
+        <v>1106175.0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="9">
@@ -4855,9 +5022,11 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>791782.0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.39658502379164</v>
+      </c>
       <c r="I8" s="2">
         <v>0</v>
       </c>
@@ -4917,10 +5086,10 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="7">
-        <v>1996500.0</v>
+        <v>1204718.0</v>
       </c>
       <c r="AJ8" s="2">
-        <v>3811500.0</v>
+        <v>2310893.0</v>
       </c>
       <c r="AK8" s="3"/>
       <c r="AL8" s="2">
@@ -4954,9 +5123,11 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>883034.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.40208273569656</v>
+      </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
@@ -5016,10 +5187,10 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="7">
-        <v>2196150.0</v>
+        <v>1313116.0</v>
       </c>
       <c r="AJ9" s="2">
-        <v>6007650.0</v>
+        <v>3624009.0</v>
       </c>
       <c r="AK9" s="3"/>
       <c r="AL9" s="2">
@@ -5053,9 +5224,11 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="3"/>
+        <v>983411.0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.40708057282062</v>
+      </c>
       <c r="I10" s="2">
         <v>0</v>
       </c>
@@ -5115,10 +5288,10 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="7">
-        <v>2415765.0</v>
+        <v>1432354.0</v>
       </c>
       <c r="AJ10" s="2">
-        <v>8423415.0</v>
+        <v>5056363.0</v>
       </c>
       <c r="AK10" s="3"/>
       <c r="AL10" s="2">
@@ -5152,9 +5325,11 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>1093826.0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.41162417401</v>
+      </c>
       <c r="I11" s="2">
         <v>0</v>
       </c>
@@ -5214,10 +5389,10 @@
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="7">
-        <v>2657341.5</v>
+        <v>1563515.5</v>
       </c>
       <c r="AJ11" s="2">
-        <v>11080756.5</v>
+        <v>6619878.5</v>
       </c>
       <c r="AK11" s="3"/>
       <c r="AL11" s="2">
@@ -5251,9 +5426,11 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>1215283.0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.41575481337093</v>
+      </c>
       <c r="I12" s="2">
         <v>0</v>
       </c>
@@ -5313,10 +5490,10 @@
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="7">
-        <v>2923076.2</v>
+        <v>1707793.2</v>
       </c>
       <c r="AJ12" s="2">
-        <v>14003832.7</v>
+        <v>8327671.7</v>
       </c>
       <c r="AK12" s="3"/>
       <c r="AL12" s="2">
@@ -5350,9 +5527,11 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>1348884.0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.41950951046712</v>
+      </c>
       <c r="I13" s="2">
         <v>0</v>
       </c>
@@ -5412,10 +5591,10 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="7">
-        <v>3215383.6</v>
+        <v>1866499.6</v>
       </c>
       <c r="AJ13" s="2">
-        <v>17219216.3</v>
+        <v>10194171.3</v>
       </c>
       <c r="AK13" s="3"/>
       <c r="AL13" s="2">
@@ -5449,9 +5628,11 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>1495846.0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.42292304744939</v>
+      </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
@@ -5511,10 +5692,10 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="7">
-        <v>3536922.4</v>
+        <v>2041076.4</v>
       </c>
       <c r="AJ14" s="2">
-        <v>20756138.7</v>
+        <v>12235247.7</v>
       </c>
       <c r="AK14" s="3"/>
       <c r="AL14" s="2">
@@ -5548,9 +5729,11 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>1657505.0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.42602656413478</v>
+      </c>
       <c r="I15" s="2">
         <v>0</v>
       </c>
@@ -5610,10 +5793,10 @@
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="7">
-        <v>3890614.2</v>
+        <v>2233109.2</v>
       </c>
       <c r="AJ15" s="2">
-        <v>24646752.9</v>
+        <v>14468356.9</v>
       </c>
       <c r="AK15" s="3"/>
       <c r="AL15" s="2">
@@ -5647,9 +5830,11 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H16" s="3"/>
+        <v>1835330.0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.42884794486984</v>
+      </c>
       <c r="I16" s="2">
         <v>0</v>
       </c>
@@ -5709,10 +5894,10 @@
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="7">
-        <v>4279675.4</v>
+        <v>2444345.4</v>
       </c>
       <c r="AJ16" s="2">
-        <v>28926428.3</v>
+        <v>16912702.3</v>
       </c>
       <c r="AK16" s="3"/>
       <c r="AL16" s="2">
@@ -5746,9 +5931,11 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H17" s="3"/>
+        <v>2030936.0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.43141253822906</v>
+      </c>
       <c r="I17" s="2">
         <v>0</v>
       </c>
@@ -5808,10 +5995,10 @@
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
       <c r="AI17" s="7">
-        <v>4707642.5</v>
+        <v>2676706.5</v>
       </c>
       <c r="AJ17" s="2">
-        <v>33634070.8</v>
+        <v>19589408.8</v>
       </c>
       <c r="AK17" s="3"/>
       <c r="AL17" s="2">
@@ -5845,9 +6032,11 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H18" s="3"/>
+        <v>2246103.0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.43374398147477</v>
+      </c>
       <c r="I18" s="2">
         <v>0</v>
       </c>
@@ -5907,10 +6096,10 @@
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="7">
-        <v>5178407.3</v>
+        <v>2932304.3</v>
       </c>
       <c r="AJ18" s="2">
-        <v>38812478.1</v>
+        <v>22521713.1</v>
       </c>
       <c r="AK18" s="3"/>
       <c r="AL18" s="2">
@@ -5944,9 +6133,11 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H19" s="3"/>
+        <v>2482788.0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.43586377046068</v>
+      </c>
       <c r="I19" s="2">
         <v>0</v>
       </c>
@@ -6006,10 +6197,10 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="7">
-        <v>5696247.7</v>
+        <v>3213459.7</v>
       </c>
       <c r="AJ19" s="2">
-        <v>44508725.8</v>
+        <v>25735172.8</v>
       </c>
       <c r="AK19" s="3"/>
       <c r="AL19" s="2">
@@ -6043,9 +6234,11 @@
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>2743141.0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.43779072565916</v>
+      </c>
       <c r="I20" s="2">
         <v>0</v>
       </c>
@@ -6105,10 +6298,10 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="7">
-        <v>6265872.8</v>
+        <v>3522731.8</v>
       </c>
       <c r="AJ20" s="2">
-        <v>50774598.6</v>
+        <v>29257904.6</v>
       </c>
       <c r="AK20" s="3"/>
       <c r="AL20" s="2">
@@ -6142,9 +6335,11 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H21" s="3"/>
+        <v>3029529.0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.43954246642523</v>
+      </c>
       <c r="I21" s="2">
         <v>0</v>
       </c>
@@ -6204,10 +6399,10 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="7">
-        <v>6892460.3</v>
+        <v>3862931.3</v>
       </c>
       <c r="AJ21" s="2">
-        <v>57667058.9</v>
+        <v>33120835.9</v>
       </c>
       <c r="AK21" s="3"/>
       <c r="AL21" s="2">
@@ -6241,9 +6436,11 @@
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H22" s="14"/>
+        <v>3344555.0</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0.44113488441783</v>
+      </c>
       <c r="I22" s="13">
         <v>0</v>
       </c>
@@ -6303,10 +6500,10 @@
       <c r="AG22" s="14"/>
       <c r="AH22" s="14"/>
       <c r="AI22" s="13">
-        <v>7581706.0</v>
+        <v>4237151.0</v>
       </c>
       <c r="AJ22" s="13">
-        <v>65248764.9</v>
+        <v>37357986.9</v>
       </c>
       <c r="AK22" s="14"/>
       <c r="AL22" s="13">
@@ -6340,9 +6537,11 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="3"/>
+        <v>3691084.0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.4425825677085</v>
+      </c>
       <c r="I23" s="2">
         <v>0</v>
       </c>
@@ -6402,10 +6601,10 @@
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
       <c r="AI23" s="7">
-        <v>8339876.6</v>
+        <v>4648792.6</v>
       </c>
       <c r="AJ23" s="2">
-        <v>73588641.5</v>
+        <v>42006779.5</v>
       </c>
       <c r="AK23" s="3"/>
       <c r="AL23" s="2">
@@ -6439,9 +6638,11 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H24" s="3"/>
+        <v>4072268.0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.44389885104802</v>
+      </c>
       <c r="I24" s="2">
         <v>0</v>
       </c>
@@ -6501,10 +6702,10 @@
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="7">
-        <v>9173864.7</v>
+        <v>5101596.7</v>
       </c>
       <c r="AJ24" s="2">
-        <v>82762506.2</v>
+        <v>47108376.2</v>
       </c>
       <c r="AK24" s="3"/>
       <c r="AL24" s="2">
@@ -6538,9 +6739,11 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>4491569.0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.44509533827395</v>
+      </c>
       <c r="I25" s="2">
         <v>0</v>
       </c>
@@ -6600,10 +6803,10 @@
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
       <c r="AI25" s="7">
-        <v>10091251.5</v>
+        <v>5599682.5</v>
       </c>
       <c r="AJ25" s="2">
-        <v>92853757.7</v>
+        <v>52708058.7</v>
       </c>
       <c r="AK25" s="3"/>
       <c r="AL25" s="2">
@@ -6637,9 +6840,11 @@
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>4952800.0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.44618303601431</v>
+      </c>
       <c r="I26" s="2">
         <v>0</v>
       </c>
@@ -6699,10 +6904,10 @@
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="7">
-        <v>11100377.2</v>
+        <v>6147577.2</v>
       </c>
       <c r="AJ26" s="2">
-        <v>103954134.9</v>
+        <v>58855635.9</v>
       </c>
       <c r="AK26" s="3"/>
       <c r="AL26" s="2">
@@ -6736,9 +6941,11 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H27" s="3"/>
+        <v>5460154.0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.44717187205771</v>
+      </c>
       <c r="I27" s="2">
         <v>0</v>
       </c>
@@ -6798,10 +7005,10 @@
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="7">
-        <v>12210414.7</v>
+        <v>6750260.7</v>
       </c>
       <c r="AJ27" s="2">
-        <v>116164549.6</v>
+        <v>65605896.6</v>
       </c>
       <c r="AK27" s="3"/>
       <c r="AL27" s="2">
@@ -6835,9 +7042,11 @@
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H28" s="3"/>
+        <v>6018242.0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.44807069136545</v>
+      </c>
       <c r="I28" s="2">
         <v>0</v>
       </c>
@@ -6897,10 +7106,10 @@
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
       <c r="AI28" s="7">
-        <v>13431456.5</v>
+        <v>7413214.5</v>
       </c>
       <c r="AJ28" s="2">
-        <v>129596006.1</v>
+        <v>73019111.1</v>
       </c>
       <c r="AK28" s="3"/>
       <c r="AL28" s="2">
@@ -6934,9 +7143,11 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="3"/>
+        <v>6632141.0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.44888794200876</v>
+      </c>
       <c r="I29" s="2">
         <v>0</v>
       </c>
@@ -6996,10 +7207,10 @@
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="7">
-        <v>14774602.7</v>
+        <v>8142461.7</v>
       </c>
       <c r="AJ29" s="2">
-        <v>144370608.8</v>
+        <v>81161572.8</v>
       </c>
       <c r="AK29" s="3"/>
       <c r="AL29" s="2">
@@ -7033,9 +7244,11 @@
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="H30" s="18"/>
+        <v>7307429.0</v>
+      </c>
+      <c r="H30" s="18">
+        <v>0.44963084779518</v>
+      </c>
       <c r="I30" s="17">
         <v>0</v>
       </c>
@@ -7095,10 +7308,10 @@
       <c r="AG30" s="18"/>
       <c r="AH30" s="18"/>
       <c r="AI30" s="17">
-        <v>16252063.3</v>
+        <v>8944634.3</v>
       </c>
       <c r="AJ30" s="17">
-        <v>160622672.1</v>
+        <v>90106207.1</v>
       </c>
       <c r="AK30" s="18"/>
       <c r="AL30" s="17">
@@ -7132,9 +7345,11 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H31" s="3"/>
+        <v>8050246.0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.45030624447773</v>
+      </c>
       <c r="I31" s="2">
         <v>0</v>
       </c>
@@ -7194,10 +7409,10 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="7">
-        <v>17877269.3</v>
+        <v>9827023.3</v>
       </c>
       <c r="AJ31" s="2">
-        <v>178499941.4</v>
+        <v>99933230.4</v>
       </c>
       <c r="AK31" s="3"/>
       <c r="AL31" s="2">
@@ -7231,9 +7446,11 @@
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>8867344.0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.45092020588725</v>
+      </c>
       <c r="I32" s="2">
         <v>0</v>
       </c>
@@ -7293,10 +7510,10 @@
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
       <c r="AI32" s="7">
-        <v>19664995.9</v>
+        <v>10797651.9</v>
       </c>
       <c r="AJ32" s="2">
-        <v>198164937.3</v>
+        <v>110730882.3</v>
       </c>
       <c r="AK32" s="3"/>
       <c r="AL32" s="2">
@@ -7330,9 +7547,11 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>9766152.0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.45147835270345</v>
+      </c>
       <c r="I33" s="2">
         <v>0</v>
       </c>
@@ -7392,10 +7611,10 @@
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="7">
-        <v>21631495.6</v>
+        <v>11865343.6</v>
       </c>
       <c r="AJ33" s="2">
-        <v>219796432.9</v>
+        <v>122596225.9</v>
       </c>
       <c r="AK33" s="3"/>
       <c r="AL33" s="2">
@@ -7429,9 +7648,11 @@
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="H34" s="18"/>
+        <v>10754842.0</v>
+      </c>
+      <c r="H34" s="18">
+        <v>0.45198580305815</v>
+      </c>
       <c r="I34" s="17">
         <v>0</v>
       </c>
@@ -7491,10 +7712,10 @@
       <c r="AG34" s="18"/>
       <c r="AH34" s="18"/>
       <c r="AI34" s="17">
-        <v>23794645.6</v>
+        <v>13039803.6</v>
       </c>
       <c r="AJ34" s="17">
-        <v>243591078.5</v>
+        <v>135636029.5</v>
       </c>
       <c r="AK34" s="18"/>
       <c r="AL34" s="17">
@@ -7528,9 +7749,11 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H35" s="3"/>
+        <v>11842400.0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.45244708334044</v>
+      </c>
       <c r="I35" s="2">
         <v>0</v>
       </c>
@@ -7590,10 +7813,10 @@
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
       <c r="AI35" s="7">
-        <v>26174110.6</v>
+        <v>14331710.6</v>
       </c>
       <c r="AJ35" s="2">
-        <v>269765189.1</v>
+        <v>149967740.1</v>
       </c>
       <c r="AK35" s="3"/>
       <c r="AL35" s="2">
@@ -7627,9 +7850,11 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H36" s="3"/>
+        <v>13038715.0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.45286647071709</v>
+      </c>
       <c r="I36" s="2">
         <v>0</v>
       </c>
@@ -7689,10 +7914,10 @@
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
       <c r="AI36" s="7">
-        <v>28791522.1</v>
+        <v>15752807.1</v>
       </c>
       <c r="AJ36" s="2">
-        <v>298556711.2</v>
+        <v>165720547.2</v>
       </c>
       <c r="AK36" s="3"/>
       <c r="AL36" s="2">
@@ -7726,9 +7951,11 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H37" s="3"/>
+        <v>14354660.0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.45324769246624</v>
+      </c>
       <c r="I37" s="2">
         <v>0</v>
       </c>
@@ -7788,10 +8015,10 @@
       <c r="AG37" s="3"/>
       <c r="AH37" s="3"/>
       <c r="AI37" s="7">
-        <v>31670674.2</v>
+        <v>17316014.2</v>
       </c>
       <c r="AJ37" s="2">
-        <v>330227385.4</v>
+        <v>183036561.4</v>
       </c>
       <c r="AK37" s="3"/>
       <c r="AL37" s="2">
@@ -7825,9 +8052,11 @@
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H38" s="3"/>
+        <v>15802199.0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0.45359424477501</v>
+      </c>
       <c r="I38" s="2">
         <v>0</v>
       </c>
@@ -7887,10 +8116,10 @@
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
       <c r="AI38" s="7">
-        <v>34837741.4</v>
+        <v>19035542.4</v>
       </c>
       <c r="AJ38" s="2">
-        <v>365065126.8</v>
+        <v>202072103.8</v>
       </c>
       <c r="AK38" s="3"/>
       <c r="AL38" s="2">
@@ -7924,9 +8153,11 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H39" s="3"/>
+        <v>17394493.0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.45390932364258</v>
+      </c>
       <c r="I39" s="2">
         <v>0</v>
       </c>
@@ -7986,10 +8217,10 @@
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
       <c r="AI39" s="7">
-        <v>38321515.1</v>
+        <v>20927022.1</v>
       </c>
       <c r="AJ39" s="2">
-        <v>403386641.9</v>
+        <v>222999125.9</v>
       </c>
       <c r="AK39" s="3"/>
       <c r="AL39" s="2">
@@ -10574,7 +10805,7 @@
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -10886,7 +11117,9 @@
       </c>
       <c r="AO6" s="2"/>
       <c r="AP6" s="3"/>
-      <c r="AQ6" s="2"/>
+      <c r="AQ6" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" spans="1:43">
       <c r="A7" s="8">
@@ -10904,9 +11137,11 @@
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="10"/>
+        <v>708825.0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.39</v>
+      </c>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
       <c r="K7" s="9"/>
@@ -10944,10 +11179,10 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="9">
-        <v>1815000.0</v>
+        <v>1106175.0</v>
       </c>
       <c r="AJ7" s="9">
-        <v>1815000.0</v>
+        <v>1106175.0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="9">
@@ -10962,7 +11197,7 @@
       <c r="AO7" s="9"/>
       <c r="AP7" s="10"/>
       <c r="AQ7" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -10981,9 +11216,11 @@
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
       <c r="G8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>791782.0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.4</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
@@ -11021,10 +11258,10 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="7">
-        <v>1996500.0</v>
+        <v>1204718.0</v>
       </c>
       <c r="AJ8" s="2">
-        <v>3811500.0</v>
+        <v>2310893.0</v>
       </c>
       <c r="AK8" s="3"/>
       <c r="AL8" s="2">
@@ -11038,7 +11275,9 @@
       </c>
       <c r="AO8" s="2"/>
       <c r="AP8" s="3"/>
-      <c r="AQ8" s="2"/>
+      <c r="AQ8" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:43">
       <c r="A9">
@@ -11056,9 +11295,11 @@
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
       <c r="G9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>883034.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.4</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
@@ -11096,10 +11337,10 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="7">
-        <v>2196150.0</v>
+        <v>1313116.0</v>
       </c>
       <c r="AJ9" s="2">
-        <v>6007650.0</v>
+        <v>3624009.0</v>
       </c>
       <c r="AK9" s="3"/>
       <c r="AL9" s="2">
@@ -11113,7 +11354,9 @@
       </c>
       <c r="AO9" s="2"/>
       <c r="AP9" s="3"/>
-      <c r="AQ9" s="2"/>
+      <c r="AQ9" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="1:43">
       <c r="A10">
@@ -11131,9 +11374,11 @@
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
       <c r="G10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="3"/>
+        <v>983411.0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.41</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
@@ -11171,10 +11416,10 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="7">
-        <v>2415765.0</v>
+        <v>1432354.0</v>
       </c>
       <c r="AJ10" s="2">
-        <v>8423415.0</v>
+        <v>5056363.0</v>
       </c>
       <c r="AK10" s="3"/>
       <c r="AL10" s="2">
@@ -11188,7 +11433,9 @@
       </c>
       <c r="AO10" s="2"/>
       <c r="AP10" s="3"/>
-      <c r="AQ10" s="2"/>
+      <c r="AQ10" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:43">
       <c r="A11">
@@ -11206,9 +11453,11 @@
       <c r="E11" s="6"/>
       <c r="F11" s="3"/>
       <c r="G11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>1093826.0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.41</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
@@ -11246,10 +11495,10 @@
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="7">
-        <v>2657341.5</v>
+        <v>1563515.5</v>
       </c>
       <c r="AJ11" s="2">
-        <v>11080756.5</v>
+        <v>6619878.5</v>
       </c>
       <c r="AK11" s="3"/>
       <c r="AL11" s="2">
@@ -11263,7 +11512,9 @@
       </c>
       <c r="AO11" s="2"/>
       <c r="AP11" s="3"/>
-      <c r="AQ11" s="2"/>
+      <c r="AQ11" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:43">
       <c r="A12">
@@ -11281,9 +11532,11 @@
       <c r="E12" s="6"/>
       <c r="F12" s="3"/>
       <c r="G12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>1215283.0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.42</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2"/>
@@ -11321,10 +11574,10 @@
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="7">
-        <v>2923076.2</v>
+        <v>1707793.2</v>
       </c>
       <c r="AJ12" s="2">
-        <v>14003832.7</v>
+        <v>8327671.7</v>
       </c>
       <c r="AK12" s="3"/>
       <c r="AL12" s="2">
@@ -11338,7 +11591,9 @@
       </c>
       <c r="AO12" s="2"/>
       <c r="AP12" s="3"/>
-      <c r="AQ12" s="2"/>
+      <c r="AQ12" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:43">
       <c r="A13">
@@ -11356,9 +11611,11 @@
       <c r="E13" s="6"/>
       <c r="F13" s="3"/>
       <c r="G13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>1348884.0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.42</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
@@ -11396,10 +11653,10 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="7">
-        <v>3215383.6</v>
+        <v>1866499.6</v>
       </c>
       <c r="AJ13" s="2">
-        <v>17219216.3</v>
+        <v>10194171.3</v>
       </c>
       <c r="AK13" s="3"/>
       <c r="AL13" s="2">
@@ -11413,7 +11670,9 @@
       </c>
       <c r="AO13" s="2"/>
       <c r="AP13" s="3"/>
-      <c r="AQ13" s="2"/>
+      <c r="AQ13" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:43">
       <c r="A14">
@@ -11431,9 +11690,11 @@
       <c r="E14" s="6"/>
       <c r="F14" s="3"/>
       <c r="G14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>1495846.0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.42</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
@@ -11471,10 +11732,10 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="7">
-        <v>3536922.4</v>
+        <v>2041076.4</v>
       </c>
       <c r="AJ14" s="2">
-        <v>20756138.7</v>
+        <v>12235247.7</v>
       </c>
       <c r="AK14" s="3"/>
       <c r="AL14" s="2">
@@ -11488,7 +11749,9 @@
       </c>
       <c r="AO14" s="2"/>
       <c r="AP14" s="3"/>
-      <c r="AQ14" s="2"/>
+      <c r="AQ14" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:43">
       <c r="A15">
@@ -11506,9 +11769,11 @@
       <c r="E15" s="6"/>
       <c r="F15" s="3"/>
       <c r="G15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>1657505.0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.43</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
@@ -11546,10 +11811,10 @@
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="7">
-        <v>3890614.2</v>
+        <v>2233109.2</v>
       </c>
       <c r="AJ15" s="2">
-        <v>24646752.9</v>
+        <v>14468356.9</v>
       </c>
       <c r="AK15" s="3"/>
       <c r="AL15" s="2">
@@ -11563,7 +11828,9 @@
       </c>
       <c r="AO15" s="2"/>
       <c r="AP15" s="3"/>
-      <c r="AQ15" s="2"/>
+      <c r="AQ15" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:43">
       <c r="A16">
@@ -11581,9 +11848,11 @@
       <c r="E16" s="6"/>
       <c r="F16" s="3"/>
       <c r="G16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H16" s="3"/>
+        <v>1835330.0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.43</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
@@ -11621,10 +11890,10 @@
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="7">
-        <v>4279675.4</v>
+        <v>2444345.4</v>
       </c>
       <c r="AJ16" s="2">
-        <v>28926428.3</v>
+        <v>16912702.3</v>
       </c>
       <c r="AK16" s="3"/>
       <c r="AL16" s="2">
@@ -11638,7 +11907,9 @@
       </c>
       <c r="AO16" s="2"/>
       <c r="AP16" s="3"/>
-      <c r="AQ16" s="2"/>
+      <c r="AQ16" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="17" spans="1:43">
       <c r="A17">
@@ -11656,9 +11927,11 @@
       <c r="E17" s="6"/>
       <c r="F17" s="3"/>
       <c r="G17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H17" s="3"/>
+        <v>2030936.0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.43</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
@@ -11696,10 +11969,10 @@
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
       <c r="AI17" s="7">
-        <v>4707642.5</v>
+        <v>2676706.5</v>
       </c>
       <c r="AJ17" s="2">
-        <v>33634070.8</v>
+        <v>19589408.8</v>
       </c>
       <c r="AK17" s="3"/>
       <c r="AL17" s="2">
@@ -11713,7 +11986,9 @@
       </c>
       <c r="AO17" s="2"/>
       <c r="AP17" s="3"/>
-      <c r="AQ17" s="2"/>
+      <c r="AQ17" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="18" spans="1:43">
       <c r="A18">
@@ -11731,9 +12006,11 @@
       <c r="E18" s="6"/>
       <c r="F18" s="3"/>
       <c r="G18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H18" s="3"/>
+        <v>2246103.0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.43</v>
+      </c>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
@@ -11771,10 +12048,10 @@
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="7">
-        <v>5178407.3</v>
+        <v>2932304.3</v>
       </c>
       <c r="AJ18" s="2">
-        <v>38812478.1</v>
+        <v>22521713.1</v>
       </c>
       <c r="AK18" s="3"/>
       <c r="AL18" s="2">
@@ -11788,7 +12065,9 @@
       </c>
       <c r="AO18" s="2"/>
       <c r="AP18" s="3"/>
-      <c r="AQ18" s="2"/>
+      <c r="AQ18" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" spans="1:43">
       <c r="A19">
@@ -11806,9 +12085,11 @@
       <c r="E19" s="6"/>
       <c r="F19" s="3"/>
       <c r="G19" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H19" s="3"/>
+        <v>2482788.0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.44</v>
+      </c>
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
@@ -11846,10 +12127,10 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="7">
-        <v>5696247.7</v>
+        <v>3213459.7</v>
       </c>
       <c r="AJ19" s="2">
-        <v>44508725.8</v>
+        <v>25735172.8</v>
       </c>
       <c r="AK19" s="3"/>
       <c r="AL19" s="2">
@@ -11863,7 +12144,9 @@
       </c>
       <c r="AO19" s="2"/>
       <c r="AP19" s="3"/>
-      <c r="AQ19" s="2"/>
+      <c r="AQ19" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="1:43">
       <c r="A20">
@@ -11881,9 +12164,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="3"/>
       <c r="G20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>2743141.0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.44</v>
+      </c>
       <c r="I20" s="2"/>
       <c r="J20" s="3"/>
       <c r="K20" s="2"/>
@@ -11921,10 +12206,10 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="7">
-        <v>6265872.8</v>
+        <v>3522731.8</v>
       </c>
       <c r="AJ20" s="2">
-        <v>50774598.6</v>
+        <v>29257904.6</v>
       </c>
       <c r="AK20" s="3"/>
       <c r="AL20" s="2">
@@ -11938,7 +12223,9 @@
       </c>
       <c r="AO20" s="2"/>
       <c r="AP20" s="3"/>
-      <c r="AQ20" s="2"/>
+      <c r="AQ20" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:43">
       <c r="A21">
@@ -11956,9 +12243,11 @@
       <c r="E21" s="6"/>
       <c r="F21" s="3"/>
       <c r="G21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H21" s="3"/>
+        <v>3029529.0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.44</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
       <c r="K21" s="2"/>
@@ -11996,10 +12285,10 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="7">
-        <v>6892460.3</v>
+        <v>3862931.3</v>
       </c>
       <c r="AJ21" s="2">
-        <v>57667058.9</v>
+        <v>33120835.9</v>
       </c>
       <c r="AK21" s="3"/>
       <c r="AL21" s="2">
@@ -12013,7 +12302,9 @@
       </c>
       <c r="AO21" s="2"/>
       <c r="AP21" s="3"/>
-      <c r="AQ21" s="2"/>
+      <c r="AQ21" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="22" spans="1:43">
       <c r="A22" s="12">
@@ -12031,9 +12322,11 @@
       <c r="E22" s="13"/>
       <c r="F22" s="14"/>
       <c r="G22" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H22" s="14"/>
+        <v>3344555.0</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0.44</v>
+      </c>
       <c r="I22" s="13"/>
       <c r="J22" s="14"/>
       <c r="K22" s="13"/>
@@ -12071,10 +12364,10 @@
       <c r="AG22" s="14"/>
       <c r="AH22" s="14"/>
       <c r="AI22" s="13">
-        <v>7581706.0</v>
+        <v>4237151.0</v>
       </c>
       <c r="AJ22" s="13">
-        <v>65248764.9</v>
+        <v>37357986.9</v>
       </c>
       <c r="AK22" s="14"/>
       <c r="AL22" s="13">
@@ -12088,7 +12381,9 @@
       </c>
       <c r="AO22" s="13"/>
       <c r="AP22" s="14"/>
-      <c r="AQ22" s="13"/>
+      <c r="AQ22" s="13" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="23" spans="1:43">
       <c r="A23">
@@ -12106,9 +12401,11 @@
       <c r="E23" s="6"/>
       <c r="F23" s="3"/>
       <c r="G23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="3"/>
+        <v>3691084.0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.44</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="3"/>
       <c r="K23" s="2"/>
@@ -12146,10 +12443,10 @@
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
       <c r="AI23" s="7">
-        <v>8339876.6</v>
+        <v>4648792.6</v>
       </c>
       <c r="AJ23" s="2">
-        <v>73588641.5</v>
+        <v>42006779.5</v>
       </c>
       <c r="AK23" s="3"/>
       <c r="AL23" s="2">
@@ -12163,7 +12460,9 @@
       </c>
       <c r="AO23" s="2"/>
       <c r="AP23" s="3"/>
-      <c r="AQ23" s="2"/>
+      <c r="AQ23" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="24" spans="1:43">
       <c r="A24">
@@ -12181,9 +12480,11 @@
       <c r="E24" s="6"/>
       <c r="F24" s="3"/>
       <c r="G24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H24" s="3"/>
+        <v>4072268.0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.44</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="3"/>
       <c r="K24" s="2"/>
@@ -12221,10 +12522,10 @@
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="7">
-        <v>9173864.7</v>
+        <v>5101596.7</v>
       </c>
       <c r="AJ24" s="2">
-        <v>82762506.2</v>
+        <v>47108376.2</v>
       </c>
       <c r="AK24" s="3"/>
       <c r="AL24" s="2">
@@ -12238,7 +12539,9 @@
       </c>
       <c r="AO24" s="2"/>
       <c r="AP24" s="3"/>
-      <c r="AQ24" s="2"/>
+      <c r="AQ24" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" spans="1:43">
       <c r="A25">
@@ -12256,9 +12559,11 @@
       <c r="E25" s="6"/>
       <c r="F25" s="3"/>
       <c r="G25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>4491569.0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="3"/>
       <c r="K25" s="2"/>
@@ -12296,10 +12601,10 @@
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
       <c r="AI25" s="7">
-        <v>10091251.5</v>
+        <v>5599682.5</v>
       </c>
       <c r="AJ25" s="2">
-        <v>92853757.7</v>
+        <v>52708058.7</v>
       </c>
       <c r="AK25" s="3"/>
       <c r="AL25" s="2">
@@ -12313,7 +12618,9 @@
       </c>
       <c r="AO25" s="2"/>
       <c r="AP25" s="3"/>
-      <c r="AQ25" s="2"/>
+      <c r="AQ25" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="26" spans="1:43">
       <c r="A26">
@@ -12331,9 +12638,11 @@
       <c r="E26" s="6"/>
       <c r="F26" s="3"/>
       <c r="G26" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>4952800.0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
       <c r="K26" s="2"/>
@@ -12371,10 +12680,10 @@
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="7">
-        <v>11100377.2</v>
+        <v>6147577.2</v>
       </c>
       <c r="AJ26" s="2">
-        <v>103954134.9</v>
+        <v>58855635.9</v>
       </c>
       <c r="AK26" s="3"/>
       <c r="AL26" s="2">
@@ -12388,7 +12697,9 @@
       </c>
       <c r="AO26" s="2"/>
       <c r="AP26" s="3"/>
-      <c r="AQ26" s="2"/>
+      <c r="AQ26" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="27" spans="1:43">
       <c r="A27">
@@ -12406,9 +12717,11 @@
       <c r="E27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H27" s="3"/>
+        <v>5460154.0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
       <c r="K27" s="2"/>
@@ -12446,10 +12759,10 @@
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="7">
-        <v>12210414.7</v>
+        <v>6750260.7</v>
       </c>
       <c r="AJ27" s="2">
-        <v>116164549.6</v>
+        <v>65605896.6</v>
       </c>
       <c r="AK27" s="3"/>
       <c r="AL27" s="2">
@@ -12463,7 +12776,9 @@
       </c>
       <c r="AO27" s="2"/>
       <c r="AP27" s="3"/>
-      <c r="AQ27" s="2"/>
+      <c r="AQ27" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="28" spans="1:43">
       <c r="A28">
@@ -12481,9 +12796,11 @@
       <c r="E28" s="6"/>
       <c r="F28" s="3"/>
       <c r="G28" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H28" s="3"/>
+        <v>6018242.0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="2"/>
@@ -12521,10 +12838,10 @@
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
       <c r="AI28" s="7">
-        <v>13431456.5</v>
+        <v>7413214.5</v>
       </c>
       <c r="AJ28" s="2">
-        <v>129596006.1</v>
+        <v>73019111.1</v>
       </c>
       <c r="AK28" s="3"/>
       <c r="AL28" s="2">
@@ -12538,7 +12855,9 @@
       </c>
       <c r="AO28" s="2"/>
       <c r="AP28" s="3"/>
-      <c r="AQ28" s="2"/>
+      <c r="AQ28" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="29" spans="1:43">
       <c r="A29">
@@ -12556,9 +12875,11 @@
       <c r="E29" s="6"/>
       <c r="F29" s="3"/>
       <c r="G29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="3"/>
+        <v>6632141.0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="2"/>
@@ -12596,10 +12917,10 @@
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="7">
-        <v>14774602.7</v>
+        <v>8142461.7</v>
       </c>
       <c r="AJ29" s="2">
-        <v>144370608.8</v>
+        <v>81161572.8</v>
       </c>
       <c r="AK29" s="3"/>
       <c r="AL29" s="2">
@@ -12613,7 +12934,9 @@
       </c>
       <c r="AO29" s="2"/>
       <c r="AP29" s="3"/>
-      <c r="AQ29" s="2"/>
+      <c r="AQ29" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="30" spans="1:43">
       <c r="A30" s="16">
@@ -12631,9 +12954,11 @@
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
       <c r="G30" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="H30" s="18"/>
+        <v>7307429.0</v>
+      </c>
+      <c r="H30" s="18">
+        <v>0.45</v>
+      </c>
       <c r="I30" s="17"/>
       <c r="J30" s="18"/>
       <c r="K30" s="17"/>
@@ -12671,10 +12996,10 @@
       <c r="AG30" s="18"/>
       <c r="AH30" s="18"/>
       <c r="AI30" s="17">
-        <v>16252063.3</v>
+        <v>8944634.3</v>
       </c>
       <c r="AJ30" s="17">
-        <v>160622672.1</v>
+        <v>90106207.1</v>
       </c>
       <c r="AK30" s="18"/>
       <c r="AL30" s="17">
@@ -12688,7 +13013,9 @@
       </c>
       <c r="AO30" s="17"/>
       <c r="AP30" s="18"/>
-      <c r="AQ30" s="17"/>
+      <c r="AQ30" s="17" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31" spans="1:43">
       <c r="A31">
@@ -12706,9 +13033,11 @@
       <c r="E31" s="6"/>
       <c r="F31" s="3"/>
       <c r="G31" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H31" s="3"/>
+        <v>8050246.0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
@@ -12746,10 +13075,10 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="7">
-        <v>17877269.3</v>
+        <v>9827023.3</v>
       </c>
       <c r="AJ31" s="2">
-        <v>178499941.4</v>
+        <v>99933230.4</v>
       </c>
       <c r="AK31" s="3"/>
       <c r="AL31" s="2">
@@ -12763,7 +13092,9 @@
       </c>
       <c r="AO31" s="2"/>
       <c r="AP31" s="3"/>
-      <c r="AQ31" s="2"/>
+      <c r="AQ31" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="32" spans="1:43">
       <c r="A32">
@@ -12781,9 +13112,11 @@
       <c r="E32" s="6"/>
       <c r="F32" s="3"/>
       <c r="G32" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>8867344.0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
       <c r="K32" s="2"/>
@@ -12821,10 +13154,10 @@
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
       <c r="AI32" s="7">
-        <v>19664995.9</v>
+        <v>10797651.9</v>
       </c>
       <c r="AJ32" s="2">
-        <v>198164937.3</v>
+        <v>110730882.3</v>
       </c>
       <c r="AK32" s="3"/>
       <c r="AL32" s="2">
@@ -12838,7 +13171,9 @@
       </c>
       <c r="AO32" s="2"/>
       <c r="AP32" s="3"/>
-      <c r="AQ32" s="2"/>
+      <c r="AQ32" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:43">
       <c r="A33">
@@ -12856,9 +13191,11 @@
       <c r="E33" s="6"/>
       <c r="F33" s="3"/>
       <c r="G33" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>9766152.0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
       <c r="K33" s="2"/>
@@ -12896,10 +13233,10 @@
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="7">
-        <v>21631495.6</v>
+        <v>11865343.6</v>
       </c>
       <c r="AJ33" s="2">
-        <v>219796432.9</v>
+        <v>122596225.9</v>
       </c>
       <c r="AK33" s="3"/>
       <c r="AL33" s="2">
@@ -12913,7 +13250,9 @@
       </c>
       <c r="AO33" s="2"/>
       <c r="AP33" s="3"/>
-      <c r="AQ33" s="2"/>
+      <c r="AQ33" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="34" spans="1:43">
       <c r="A34" s="16">
@@ -12931,9 +13270,11 @@
       <c r="E34" s="17"/>
       <c r="F34" s="18"/>
       <c r="G34" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="H34" s="18"/>
+        <v>10754842.0</v>
+      </c>
+      <c r="H34" s="18">
+        <v>0.45</v>
+      </c>
       <c r="I34" s="17"/>
       <c r="J34" s="18"/>
       <c r="K34" s="17"/>
@@ -12971,10 +13312,10 @@
       <c r="AG34" s="18"/>
       <c r="AH34" s="18"/>
       <c r="AI34" s="17">
-        <v>23794645.6</v>
+        <v>13039803.6</v>
       </c>
       <c r="AJ34" s="17">
-        <v>243591078.5</v>
+        <v>135636029.5</v>
       </c>
       <c r="AK34" s="18"/>
       <c r="AL34" s="17">
@@ -12988,7 +13329,9 @@
       </c>
       <c r="AO34" s="17"/>
       <c r="AP34" s="18"/>
-      <c r="AQ34" s="17"/>
+      <c r="AQ34" s="17" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="35" spans="1:43">
       <c r="A35">
@@ -13006,9 +13349,11 @@
       <c r="E35" s="6"/>
       <c r="F35" s="3"/>
       <c r="G35" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H35" s="3"/>
+        <v>11842400.0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I35" s="2"/>
       <c r="J35" s="3"/>
       <c r="K35" s="2"/>
@@ -13046,10 +13391,10 @@
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
       <c r="AI35" s="7">
-        <v>26174110.6</v>
+        <v>14331710.6</v>
       </c>
       <c r="AJ35" s="2">
-        <v>269765189.1</v>
+        <v>149967740.1</v>
       </c>
       <c r="AK35" s="3"/>
       <c r="AL35" s="2">
@@ -13063,7 +13408,9 @@
       </c>
       <c r="AO35" s="2"/>
       <c r="AP35" s="3"/>
-      <c r="AQ35" s="2"/>
+      <c r="AQ35" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="36" spans="1:43">
       <c r="A36">
@@ -13081,9 +13428,11 @@
       <c r="E36" s="6"/>
       <c r="F36" s="3"/>
       <c r="G36" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H36" s="3"/>
+        <v>13038715.0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I36" s="2"/>
       <c r="J36" s="3"/>
       <c r="K36" s="2"/>
@@ -13121,10 +13470,10 @@
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
       <c r="AI36" s="7">
-        <v>28791522.1</v>
+        <v>15752807.1</v>
       </c>
       <c r="AJ36" s="2">
-        <v>298556711.2</v>
+        <v>165720547.2</v>
       </c>
       <c r="AK36" s="3"/>
       <c r="AL36" s="2">
@@ -13138,7 +13487,9 @@
       </c>
       <c r="AO36" s="2"/>
       <c r="AP36" s="3"/>
-      <c r="AQ36" s="2"/>
+      <c r="AQ36" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="37" spans="1:43">
       <c r="A37">
@@ -13156,9 +13507,11 @@
       <c r="E37" s="6"/>
       <c r="F37" s="3"/>
       <c r="G37" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H37" s="3"/>
+        <v>14354660.0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
       <c r="K37" s="2"/>
@@ -13196,10 +13549,10 @@
       <c r="AG37" s="3"/>
       <c r="AH37" s="3"/>
       <c r="AI37" s="7">
-        <v>31670674.2</v>
+        <v>17316014.2</v>
       </c>
       <c r="AJ37" s="2">
-        <v>330227385.4</v>
+        <v>183036561.4</v>
       </c>
       <c r="AK37" s="3"/>
       <c r="AL37" s="2">
@@ -13213,7 +13566,9 @@
       </c>
       <c r="AO37" s="2"/>
       <c r="AP37" s="3"/>
-      <c r="AQ37" s="2"/>
+      <c r="AQ37" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="38" spans="1:43">
       <c r="A38">
@@ -13231,9 +13586,11 @@
       <c r="E38" s="6"/>
       <c r="F38" s="3"/>
       <c r="G38" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H38" s="3"/>
+        <v>15802199.0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I38" s="2"/>
       <c r="J38" s="3"/>
       <c r="K38" s="2"/>
@@ -13271,10 +13628,10 @@
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
       <c r="AI38" s="7">
-        <v>34837741.4</v>
+        <v>19035542.4</v>
       </c>
       <c r="AJ38" s="2">
-        <v>365065126.8</v>
+        <v>202072103.8</v>
       </c>
       <c r="AK38" s="3"/>
       <c r="AL38" s="2">
@@ -13288,7 +13645,9 @@
       </c>
       <c r="AO38" s="2"/>
       <c r="AP38" s="3"/>
-      <c r="AQ38" s="2"/>
+      <c r="AQ38" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="39" spans="1:43">
       <c r="A39">
@@ -13306,9 +13665,11 @@
       <c r="E39" s="6"/>
       <c r="F39" s="3"/>
       <c r="G39" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H39" s="3"/>
+        <v>17394493.0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.45</v>
+      </c>
       <c r="I39" s="2"/>
       <c r="J39" s="3"/>
       <c r="K39" s="2"/>
@@ -13346,10 +13707,10 @@
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
       <c r="AI39" s="7">
-        <v>38321515.1</v>
+        <v>20927022.1</v>
       </c>
       <c r="AJ39" s="2">
-        <v>403386641.9</v>
+        <v>222999125.9</v>
       </c>
       <c r="AK39" s="3"/>
       <c r="AL39" s="2">
@@ -13363,7 +13724,9 @@
       </c>
       <c r="AO39" s="2"/>
       <c r="AP39" s="3"/>
-      <c r="AQ39" s="2"/>
+      <c r="AQ39" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="40" spans="1:43">
       <c r="C40" s="20"/>

</xml_diff>